<commit_message>
running in my computer
</commit_message>
<xml_diff>
--- a/xls/result.xlsx
+++ b/xls/result.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="表1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,62 +12,6 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
-  <si>
-    <t>序号</t>
-  </si>
-  <si>
-    <t>CPU</t>
-  </si>
-  <si>
-    <t>内存</t>
-  </si>
-  <si>
-    <t>显卡</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>Intel</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>DDR3</t>
-  </si>
-  <si>
-    <t>DDR4</t>
-  </si>
-  <si>
-    <t>NVIDIA</t>
-  </si>
-  <si>
-    <t>集成</t>
-  </si>
-  <si>
-    <t>i7-8650U</t>
-  </si>
-  <si>
-    <t>16GB</t>
-  </si>
-  <si>
-    <t>UHD620</t>
-  </si>
-  <si>
-    <t>i5-4200H</t>
-  </si>
-  <si>
-    <t>12GB</t>
-  </si>
-  <si>
-    <t>GF-745M</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -182,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -207,106 +151,185 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="00000000"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="5" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="6" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="8" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -607,91 +630,127 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>序号</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>CPU</t>
+        </is>
       </c>
       <c r="E1" s="3" t="n"/>
-      <c r="F1" s="4" t="s">
-        <v>2</v>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>内存</t>
+        </is>
       </c>
       <c r="G1" s="3" t="n"/>
-      <c r="H1" s="5" t="s">
-        <v>3</v>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>显卡</t>
+        </is>
       </c>
       <c r="I1" s="6" t="n"/>
       <c r="J1" s="3" t="n"/>
-      <c r="K1" s="7" t="s">
-        <v>4</v>
+      <c r="K1" s="7" t="inlineStr">
+        <is>
+          <t>备注</t>
+        </is>
       </c>
       <c r="L1" s="8" t="n"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2">
       <c r="C2" s="9" t="n"/>
-      <c r="D2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>10</v>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="F2" s="11" t="inlineStr">
+        <is>
+          <t>DDR3</t>
+        </is>
+      </c>
+      <c r="G2" s="11" t="inlineStr">
+        <is>
+          <t>DDR4</t>
+        </is>
+      </c>
+      <c r="H2" s="12" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="I2" s="12" t="inlineStr">
+        <is>
+          <t>NVIDIA</t>
+        </is>
+      </c>
+      <c r="J2" s="13" t="inlineStr">
+        <is>
+          <t>集成</t>
+        </is>
       </c>
       <c r="K2" s="9" t="n"/>
       <c r="L2" s="8" t="n"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3">
       <c r="C3" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>11</v>
+      <c r="D3" s="14" t="inlineStr">
+        <is>
+          <t>i7-8650U</t>
+        </is>
       </c>
       <c r="E3" s="14" t="n"/>
       <c r="F3" s="15" t="n"/>
-      <c r="G3" s="15" t="s">
-        <v>12</v>
+      <c r="G3" s="15" t="inlineStr">
+        <is>
+          <t>16GB</t>
+        </is>
       </c>
       <c r="H3" s="15" t="n"/>
       <c r="I3" s="15" t="n"/>
-      <c r="J3" s="15" t="s">
-        <v>13</v>
+      <c r="J3" s="15" t="inlineStr">
+        <is>
+          <t>UHD620</t>
+        </is>
       </c>
       <c r="K3" s="15" t="n">
         <v>0</v>
       </c>
       <c r="L3" s="15" t="n"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4">
       <c r="C4" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>14</v>
+      <c r="D4" s="15" t="inlineStr">
+        <is>
+          <t>i5-4200H</t>
+        </is>
       </c>
       <c r="E4" s="15" t="n"/>
       <c r="F4" s="15" t="n"/>
-      <c r="G4" s="15" t="s">
-        <v>15</v>
+      <c r="G4" s="15" t="inlineStr">
+        <is>
+          <t>12GB</t>
+        </is>
       </c>
       <c r="H4" s="15" t="n"/>
-      <c r="I4" s="15" t="s">
-        <v>16</v>
+      <c r="I4" s="15" t="inlineStr">
+        <is>
+          <t>GF-745M</t>
+        </is>
       </c>
       <c r="J4" s="15" t="n"/>
       <c r="K4" s="15" t="n">
@@ -707,6 +766,6 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>